<commit_message>
update CV page with printing
</commit_message>
<xml_diff>
--- a/_site/content-excel.xlsx
+++ b/_site/content-excel.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ha8343al\GitHub\Alsafadi.github.io\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF8128DA-6CD9-4FBE-BA72-F1D62AF084CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE60937C-16ED-4935-BC6E-A5AA798F4AEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="32145" yWindow="4035" windowWidth="38700" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11160" yWindow="1845" windowWidth="38700" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="content" sheetId="1" r:id="rId1"/>
@@ -20,13 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="380" uniqueCount="212">
-  <si>
-    <t>section</t>
-  </si>
-  <si>
-    <t>display</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="502" uniqueCount="238">
   <si>
     <t>itemid</t>
   </si>
@@ -58,9 +52,6 @@
     <t>Eduction</t>
   </si>
   <si>
-    <t>Current</t>
-  </si>
-  <si>
     <t>Lund University</t>
   </si>
   <si>
@@ -73,9 +64,6 @@
     <t>Sweden</t>
   </si>
   <si>
-    <t>(Half-time passed: 2020.10.28)</t>
-  </si>
-  <si>
     <t>Comprehensive Pneumology Center (CPC)</t>
   </si>
   <si>
@@ -166,9 +154,6 @@
     <t>Select Research Experience</t>
   </si>
   <si>
-    <t>Present</t>
-  </si>
-  <si>
     <t>Experimental Medical Sciences, Lung bioengineering and regeneration</t>
   </si>
   <si>
@@ -229,9 +214,6 @@
     <t>Publications</t>
   </si>
   <si>
-    <t>Research Supervision</t>
-  </si>
-  <si>
     <t>Spain</t>
   </si>
   <si>
@@ -265,9 +247,6 @@
     <t xml:space="preserve">Eliora Sy Wee </t>
   </si>
   <si>
-    <t>Invited talks</t>
-  </si>
-  <si>
     <t>Role of Hippo signaling and Yap/Taz in the Lung Epithelium during Fibrosis</t>
   </si>
   <si>
@@ -418,9 +397,6 @@
     <t>Italian</t>
   </si>
   <si>
-    <t>Beginner</t>
-  </si>
-  <si>
     <t>Swedish</t>
   </si>
   <si>
@@ -448,9 +424,6 @@
     <t>Linköping</t>
   </si>
   <si>
-    <t>08.201</t>
-  </si>
-  <si>
     <t>05.2010</t>
   </si>
   <si>
@@ -613,9 +586,6 @@
     <t>Python</t>
   </si>
   <si>
-    <t>Statistis; Omics analysis and Intergration; RNAseq; Single cell RNASeq; Data visualization using ggplot2 and plotly</t>
-  </si>
-  <si>
     <t>Genomic analysis tools; Singel Cell RNAseq; Data visualization with matplotlib and seaborn</t>
   </si>
   <si>
@@ -634,9 +604,6 @@
     <t>Web application development and intergration with SQL</t>
   </si>
   <si>
-    <t>Select Developer/Analytical Skills</t>
-  </si>
-  <si>
     <t>IJMacro</t>
   </si>
   <si>
@@ -656,13 +623,287 @@
   </si>
   <si>
     <t>Static webpage development</t>
+  </si>
+  <si>
+    <t>print</t>
+  </si>
+  <si>
+    <t>printable</t>
+  </si>
+  <si>
+    <t>02.2023</t>
+  </si>
+  <si>
+    <t>11.2017</t>
+  </si>
+  <si>
+    <t>Select Bioinformatics Skills</t>
+  </si>
+  <si>
+    <t>Select Research Skills</t>
+  </si>
+  <si>
+    <t>3D culture models</t>
+  </si>
+  <si>
+    <t>PCLS, Lung organoids</t>
+  </si>
+  <si>
+    <t>Advanced Microcopy techniques</t>
+  </si>
+  <si>
+    <t>Lightsheet microscopy, Confocal microscopy, SEM</t>
+  </si>
+  <si>
+    <t>Primary cell isolation</t>
+  </si>
+  <si>
+    <t>Human and murine distal and proximal lung epithelial cells</t>
+  </si>
+  <si>
+    <t>12.2017</t>
+  </si>
+  <si>
+    <t>11.2015</t>
+  </si>
+  <si>
+    <t>10.2017</t>
+  </si>
+  <si>
+    <t>12.2014</t>
+  </si>
+  <si>
+    <t>Development of in vitro assays</t>
+  </si>
+  <si>
+    <t>In vitro assay for studying matrix remodelling</t>
+  </si>
+  <si>
+    <t>Role of the co-transcriptional regulators Yap/Taz in the normal and fibrotic lung epithelia</t>
+  </si>
+  <si>
+    <t>Irene Urrecho</t>
+  </si>
+  <si>
+    <t>Select Research Supervision</t>
+  </si>
+  <si>
+    <t>CUT&amp;RUN</t>
+  </si>
+  <si>
+    <t>European Molecular Imaging Meeting</t>
+  </si>
+  <si>
+    <t>Thessaloniki</t>
+  </si>
+  <si>
+    <t>Greece</t>
+  </si>
+  <si>
+    <t>Oral Presentation</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">inFLATION: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10.5"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t>IN</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">fusion of </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10.5"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t>F</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t>luorescent </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10.5"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t>L</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t>abelled</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10.5"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t>A</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t>ntibodies in </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10.5"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t>T</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">issue of </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10.5"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t>I</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">ntact </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10.5"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t>O</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t>rga</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10.5"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t>N</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t>s</t>
+    </r>
+  </si>
+  <si>
+    <t>Select Invited Talks</t>
+  </si>
+  <si>
+    <t>Lund Respiratory Network (LURN)</t>
+  </si>
+  <si>
+    <t>12.2021</t>
+  </si>
+  <si>
+    <t>12.2022</t>
+  </si>
+  <si>
+    <t>Section</t>
+  </si>
+  <si>
+    <t>"Thesis title: Role of the co-transcriptional regulators Yap/Taz in the normal and fibrotic lung epithelia"</t>
+  </si>
+  <si>
+    <t>Statistics; Omics analysis and Intergration; RNAseq; Single cell RNASeq; Data visualization using ggplot2 and plotly</t>
+  </si>
+  <si>
+    <t>08.2010</t>
+  </si>
+  <si>
+    <t>Intermediate</t>
+  </si>
+  <si>
+    <t>hideit</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -796,6 +1037,25 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10.5"/>
+      <color theme="1"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10.5"/>
+      <color theme="1"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="33">
@@ -1139,8 +1399,12 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1496,16 +1760,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L79"/>
+  <dimension ref="A1:L86"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="35.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.28515625" customWidth="1"/>
+    <col min="3" max="3" width="11.7109375" customWidth="1"/>
     <col min="7" max="7" width="58.28515625" customWidth="1"/>
     <col min="8" max="8" width="65" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="21.5703125" bestFit="1" customWidth="1"/>
@@ -1516,167 +1781,182 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>232</v>
+      </c>
+      <c r="B1" t="s">
+        <v>177</v>
+      </c>
+      <c r="C1" t="s">
+        <v>202</v>
+      </c>
+      <c r="D1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
-        <v>186</v>
-      </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" t="s">
+      <c r="J1" t="s">
         <v>6</v>
       </c>
-      <c r="I1" t="s">
+      <c r="K1" t="s">
         <v>7</v>
       </c>
-      <c r="J1" t="s">
+      <c r="L1" t="s">
         <v>8</v>
-      </c>
-      <c r="K1" t="s">
-        <v>9</v>
-      </c>
-      <c r="L1" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B2" t="s">
-        <v>187</v>
+        <v>178</v>
+      </c>
+      <c r="C2" t="s">
+        <v>201</v>
       </c>
       <c r="D2">
         <v>1</v>
       </c>
-      <c r="E2" t="s">
-        <v>146</v>
+      <c r="E2" s="2" t="s">
+        <v>137</v>
       </c>
       <c r="F2" t="s">
+        <v>203</v>
+      </c>
+      <c r="G2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H2" t="s">
+        <v>11</v>
+      </c>
+      <c r="I2" t="s">
         <v>12</v>
       </c>
-      <c r="G2" t="s">
+      <c r="J2" t="s">
         <v>13</v>
       </c>
-      <c r="H2" t="s">
-        <v>14</v>
-      </c>
-      <c r="I2" t="s">
-        <v>15</v>
-      </c>
-      <c r="J2" t="s">
-        <v>16</v>
-      </c>
       <c r="K2" t="s">
-        <v>17</v>
+        <v>233</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B3" t="s">
-        <v>187</v>
+        <v>178</v>
+      </c>
+      <c r="C3" t="s">
+        <v>201</v>
       </c>
       <c r="D3">
         <v>2</v>
       </c>
       <c r="E3" t="s">
-        <v>145</v>
-      </c>
-      <c r="F3">
-        <v>11.201700000000001</v>
+        <v>136</v>
+      </c>
+      <c r="F3" t="s">
+        <v>204</v>
       </c>
       <c r="G3" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="H3" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="I3" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="J3" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B4" t="s">
-        <v>187</v>
+        <v>178</v>
+      </c>
+      <c r="C4" t="s">
+        <v>201</v>
       </c>
       <c r="D4">
         <v>3</v>
       </c>
-      <c r="E4" t="s">
-        <v>142</v>
+      <c r="E4" s="2" t="s">
+        <v>235</v>
       </c>
       <c r="F4" t="s">
-        <v>147</v>
+        <v>138</v>
       </c>
       <c r="G4" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="H4" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="I4" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="J4" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B5" t="s">
-        <v>187</v>
+        <v>178</v>
+      </c>
+      <c r="C5" t="s">
+        <v>201</v>
       </c>
       <c r="D5">
         <v>4</v>
       </c>
       <c r="E5" t="s">
-        <v>144</v>
+        <v>135</v>
       </c>
       <c r="F5" t="s">
-        <v>143</v>
+        <v>134</v>
       </c>
       <c r="G5" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="H5" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="I5" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="J5" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="B6" t="s">
-        <v>187</v>
+        <v>178</v>
+      </c>
+      <c r="C6" t="s">
+        <v>201</v>
       </c>
       <c r="D6">
         <v>1</v>
@@ -1685,27 +1965,30 @@
         <v>2021</v>
       </c>
       <c r="G6" t="s">
-        <v>189</v>
+        <v>180</v>
       </c>
       <c r="H6" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="I6" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="J6" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="K6" t="s">
-        <v>190</v>
+        <v>181</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="B7" t="s">
-        <v>187</v>
+        <v>178</v>
+      </c>
+      <c r="C7" t="s">
+        <v>201</v>
       </c>
       <c r="D7">
         <v>2</v>
@@ -1714,27 +1997,30 @@
         <v>2017</v>
       </c>
       <c r="G7" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="H7" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="I7" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="J7" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="K7" t="s">
-        <v>192</v>
+        <v>183</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="B8" t="s">
-        <v>187</v>
+        <v>178</v>
+      </c>
+      <c r="C8" t="s">
+        <v>237</v>
       </c>
       <c r="D8">
         <v>3</v>
@@ -1746,27 +2032,30 @@
         <v>2014</v>
       </c>
       <c r="G8" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="H8" t="s">
-        <v>193</v>
+        <v>184</v>
       </c>
       <c r="I8" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="J8" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="K8" t="s">
-        <v>191</v>
+        <v>182</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="B9" t="s">
-        <v>187</v>
+        <v>178</v>
+      </c>
+      <c r="C9" t="s">
+        <v>237</v>
       </c>
       <c r="D9">
         <v>4</v>
@@ -1778,27 +2067,30 @@
         <v>2010</v>
       </c>
       <c r="G9" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="H9" t="s">
-        <v>193</v>
+        <v>184</v>
       </c>
       <c r="I9" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="J9" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="K9" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="B10" t="s">
-        <v>187</v>
+        <v>178</v>
+      </c>
+      <c r="C10" t="s">
+        <v>201</v>
       </c>
       <c r="D10">
         <v>5</v>
@@ -1807,27 +2099,30 @@
         <v>2018</v>
       </c>
       <c r="G10" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="H10" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="I10" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="J10" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="K10" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="B11" t="s">
-        <v>187</v>
+        <v>178</v>
+      </c>
+      <c r="C11" t="s">
+        <v>201</v>
       </c>
       <c r="D11">
         <v>6</v>
@@ -1836,27 +2131,30 @@
         <v>2021</v>
       </c>
       <c r="G11" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="H11" t="s">
-        <v>188</v>
+        <v>179</v>
       </c>
       <c r="I11" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="J11" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="K11" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="B12" t="s">
-        <v>187</v>
+        <v>178</v>
+      </c>
+      <c r="C12" t="s">
+        <v>201</v>
       </c>
       <c r="D12">
         <v>7</v>
@@ -1865,24 +2163,27 @@
         <v>2020</v>
       </c>
       <c r="G12" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="H12" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="I12" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="J12" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="B13" t="s">
-        <v>187</v>
+        <v>178</v>
+      </c>
+      <c r="C13" t="s">
+        <v>201</v>
       </c>
       <c r="D13">
         <v>8</v>
@@ -1891,24 +2192,27 @@
         <v>2019</v>
       </c>
       <c r="G13" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="H13" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="I13" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="J13" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="B14" t="s">
-        <v>187</v>
+        <v>178</v>
+      </c>
+      <c r="C14" t="s">
+        <v>237</v>
       </c>
       <c r="D14">
         <v>9</v>
@@ -1917,1179 +2221,1519 @@
         <v>2019</v>
       </c>
       <c r="G14" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="H14" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="I14" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="J14" t="s">
-        <v>16</v>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>205</v>
+      </c>
+      <c r="C15" t="s">
+        <v>201</v>
+      </c>
+      <c r="G15" t="s">
+        <v>186</v>
+      </c>
+      <c r="H15" t="s">
+        <v>234</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>204</v>
+        <v>205</v>
+      </c>
+      <c r="C16" t="s">
+        <v>201</v>
       </c>
       <c r="G16" t="s">
-        <v>195</v>
+        <v>187</v>
       </c>
       <c r="H16" t="s">
-        <v>197</v>
+        <v>188</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>204</v>
+        <v>205</v>
+      </c>
+      <c r="C17" t="s">
+        <v>201</v>
       </c>
       <c r="G17" t="s">
-        <v>196</v>
+        <v>189</v>
       </c>
       <c r="H17" t="s">
-        <v>198</v>
+        <v>190</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>204</v>
+        <v>205</v>
+      </c>
+      <c r="C18" t="s">
+        <v>201</v>
       </c>
       <c r="G18" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
       <c r="H18" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>204</v>
+        <v>205</v>
+      </c>
+      <c r="C19" t="s">
+        <v>237</v>
       </c>
       <c r="G19" t="s">
-        <v>205</v>
+        <v>191</v>
       </c>
       <c r="H19" t="s">
-        <v>206</v>
+        <v>196</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>204</v>
+        <v>205</v>
+      </c>
+      <c r="C20" t="s">
+        <v>237</v>
       </c>
       <c r="G20" t="s">
-        <v>201</v>
+        <v>192</v>
       </c>
       <c r="H20" t="s">
-        <v>207</v>
+        <v>193</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>204</v>
+        <v>205</v>
+      </c>
+      <c r="C21" t="s">
+        <v>237</v>
       </c>
       <c r="G21" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="H21" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>204</v>
+        <v>205</v>
+      </c>
+      <c r="C22" t="s">
+        <v>237</v>
       </c>
       <c r="G22" t="s">
-        <v>208</v>
+        <v>199</v>
       </c>
       <c r="H22" t="s">
-        <v>209</v>
+        <v>200</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>204</v>
+        <v>206</v>
+      </c>
+      <c r="C23" t="s">
+        <v>201</v>
       </c>
       <c r="G23" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="H23" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>47</v>
-      </c>
-      <c r="B24" t="s">
-        <v>194</v>
-      </c>
-      <c r="D24">
-        <v>1</v>
-      </c>
-      <c r="E24" t="s">
-        <v>146</v>
-      </c>
-      <c r="F24" t="s">
-        <v>48</v>
+        <v>206</v>
+      </c>
+      <c r="C24" t="s">
+        <v>201</v>
       </c>
       <c r="G24" t="s">
-        <v>13</v>
+        <v>209</v>
       </c>
       <c r="H24" t="s">
-        <v>49</v>
-      </c>
-      <c r="I24" t="s">
-        <v>15</v>
-      </c>
-      <c r="J24" t="s">
-        <v>16</v>
-      </c>
-      <c r="K24" t="s">
-        <v>50</v>
+        <v>210</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>47</v>
-      </c>
-      <c r="B25" t="s">
-        <v>194</v>
-      </c>
-      <c r="D25">
-        <v>2</v>
-      </c>
-      <c r="E25">
-        <v>12.201700000000001</v>
-      </c>
-      <c r="F25" t="s">
-        <v>146</v>
+        <v>206</v>
+      </c>
+      <c r="C25" t="s">
+        <v>201</v>
       </c>
       <c r="G25" t="s">
-        <v>13</v>
+        <v>211</v>
       </c>
       <c r="H25" t="s">
-        <v>49</v>
-      </c>
-      <c r="I25" t="s">
-        <v>15</v>
-      </c>
-      <c r="J25" t="s">
-        <v>16</v>
-      </c>
-      <c r="K25" t="s">
-        <v>51</v>
-      </c>
-      <c r="L25" t="s">
-        <v>52</v>
+        <v>212</v>
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>47</v>
-      </c>
-      <c r="B26" t="s">
-        <v>194</v>
-      </c>
-      <c r="D26">
-        <v>3</v>
-      </c>
-      <c r="E26">
-        <v>11.201499999999999</v>
-      </c>
-      <c r="F26">
-        <v>11.201700000000001</v>
+        <v>206</v>
+      </c>
+      <c r="C26" t="s">
+        <v>201</v>
       </c>
       <c r="G26" t="s">
-        <v>53</v>
+        <v>217</v>
       </c>
       <c r="H26" t="s">
-        <v>54</v>
-      </c>
-      <c r="I26" t="s">
-        <v>20</v>
-      </c>
-      <c r="J26" t="s">
-        <v>21</v>
-      </c>
-      <c r="K26" t="s">
-        <v>55</v>
-      </c>
-      <c r="L26" t="s">
-        <v>56</v>
+        <v>218</v>
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B27" t="s">
-        <v>194</v>
+        <v>185</v>
+      </c>
+      <c r="C27" t="s">
+        <v>201</v>
       </c>
       <c r="D27">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E27" t="s">
-        <v>151</v>
-      </c>
-      <c r="F27">
-        <v>10.201700000000001</v>
+        <v>137</v>
+      </c>
+      <c r="F27" t="s">
+        <v>203</v>
       </c>
       <c r="G27" t="s">
+        <v>10</v>
+      </c>
+      <c r="H27" t="s">
+        <v>44</v>
+      </c>
+      <c r="I27" t="s">
+        <v>12</v>
+      </c>
+      <c r="J27" t="s">
         <v>13</v>
       </c>
-      <c r="H27" t="s">
-        <v>57</v>
-      </c>
-      <c r="I27" t="s">
-        <v>15</v>
-      </c>
-      <c r="J27" t="s">
-        <v>16</v>
-      </c>
       <c r="K27" t="s">
-        <v>58</v>
+        <v>45</v>
       </c>
       <c r="L27" t="s">
-        <v>59</v>
+        <v>219</v>
       </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
+        <v>43</v>
+      </c>
+      <c r="B28" t="s">
+        <v>185</v>
+      </c>
+      <c r="C28" t="s">
+        <v>201</v>
+      </c>
+      <c r="D28">
+        <v>2</v>
+      </c>
+      <c r="E28" t="s">
+        <v>213</v>
+      </c>
+      <c r="F28" t="s">
+        <v>137</v>
+      </c>
+      <c r="G28" t="s">
+        <v>10</v>
+      </c>
+      <c r="H28" t="s">
+        <v>44</v>
+      </c>
+      <c r="I28" t="s">
+        <v>12</v>
+      </c>
+      <c r="J28" t="s">
+        <v>13</v>
+      </c>
+      <c r="K28" t="s">
+        <v>46</v>
+      </c>
+      <c r="L28" t="s">
         <v>47</v>
-      </c>
-      <c r="B28" t="s">
-        <v>194</v>
-      </c>
-      <c r="D28">
-        <v>5</v>
-      </c>
-      <c r="E28" t="s">
-        <v>150</v>
-      </c>
-      <c r="F28" t="s">
-        <v>148</v>
-      </c>
-      <c r="G28" t="s">
-        <v>60</v>
-      </c>
-      <c r="H28" t="s">
-        <v>61</v>
-      </c>
-      <c r="I28" t="s">
-        <v>15</v>
-      </c>
-      <c r="J28" t="s">
-        <v>16</v>
-      </c>
-      <c r="K28" t="s">
-        <v>58</v>
-      </c>
-      <c r="L28" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B29" t="s">
-        <v>194</v>
+        <v>185</v>
+      </c>
+      <c r="C29" t="s">
+        <v>201</v>
       </c>
       <c r="D29">
-        <v>6</v>
-      </c>
-      <c r="E29">
-        <v>12.2014</v>
+        <v>3</v>
+      </c>
+      <c r="E29" t="s">
+        <v>214</v>
       </c>
       <c r="F29" t="s">
-        <v>149</v>
+        <v>204</v>
       </c>
       <c r="G29" t="s">
-        <v>63</v>
+        <v>48</v>
       </c>
       <c r="H29" t="s">
-        <v>64</v>
+        <v>49</v>
       </c>
       <c r="I29" t="s">
-        <v>65</v>
+        <v>16</v>
       </c>
       <c r="J29" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="K29" t="s">
-        <v>66</v>
+        <v>50</v>
       </c>
       <c r="L29" t="s">
-        <v>67</v>
+        <v>51</v>
       </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>68</v>
+        <v>43</v>
+      </c>
+      <c r="B30" t="s">
+        <v>185</v>
+      </c>
+      <c r="C30" t="s">
+        <v>201</v>
       </c>
       <c r="D30">
-        <v>1</v>
+        <v>4</v>
+      </c>
+      <c r="E30" t="s">
+        <v>142</v>
+      </c>
+      <c r="F30" t="s">
+        <v>215</v>
+      </c>
+      <c r="G30" t="s">
+        <v>10</v>
+      </c>
+      <c r="H30" t="s">
+        <v>52</v>
+      </c>
+      <c r="I30" t="s">
+        <v>12</v>
+      </c>
+      <c r="J30" t="s">
+        <v>13</v>
+      </c>
+      <c r="K30" t="s">
+        <v>53</v>
+      </c>
+      <c r="L30" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>69</v>
+        <v>43</v>
+      </c>
+      <c r="B31" t="s">
+        <v>185</v>
+      </c>
+      <c r="C31" t="s">
+        <v>237</v>
       </c>
       <c r="D31">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E31" t="s">
+        <v>141</v>
+      </c>
+      <c r="F31" t="s">
+        <v>139</v>
+      </c>
+      <c r="G31" t="s">
+        <v>55</v>
+      </c>
+      <c r="H31" t="s">
+        <v>56</v>
+      </c>
+      <c r="I31" t="s">
         <v>12</v>
       </c>
-      <c r="G31" t="s">
-        <v>139</v>
-      </c>
       <c r="J31" t="s">
-        <v>70</v>
+        <v>13</v>
       </c>
       <c r="K31" t="s">
-        <v>71</v>
+        <v>53</v>
+      </c>
+      <c r="L31" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>69</v>
+        <v>43</v>
+      </c>
+      <c r="B32" t="s">
+        <v>185</v>
+      </c>
+      <c r="C32" t="s">
+        <v>201</v>
       </c>
       <c r="D32">
-        <v>2</v>
-      </c>
-      <c r="E32">
-        <v>2021</v>
+        <v>6</v>
+      </c>
+      <c r="E32" t="s">
+        <v>216</v>
+      </c>
+      <c r="F32" t="s">
+        <v>140</v>
       </c>
       <c r="G32" t="s">
-        <v>72</v>
+        <v>58</v>
+      </c>
+      <c r="H32" t="s">
+        <v>59</v>
+      </c>
+      <c r="I32" t="s">
+        <v>60</v>
       </c>
       <c r="J32" t="s">
-        <v>73</v>
+        <v>21</v>
       </c>
       <c r="K32" t="s">
-        <v>71</v>
+        <v>61</v>
+      </c>
+      <c r="L32" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>69</v>
-      </c>
-      <c r="D33">
-        <v>3</v>
-      </c>
-      <c r="E33">
-        <v>2021</v>
-      </c>
-      <c r="G33" t="s">
-        <v>74</v>
-      </c>
-      <c r="J33" t="s">
-        <v>70</v>
-      </c>
-      <c r="K33" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>69</v>
+        <v>221</v>
+      </c>
+      <c r="C34" t="s">
+        <v>201</v>
       </c>
       <c r="D34">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E34">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="G34" t="s">
-        <v>75</v>
+        <v>220</v>
       </c>
       <c r="J34" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="K34" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>69</v>
+        <v>221</v>
+      </c>
+      <c r="C35" t="s">
+        <v>201</v>
       </c>
       <c r="D35">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E35">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="G35" t="s">
-        <v>76</v>
+        <v>131</v>
       </c>
       <c r="J35" t="s">
-        <v>77</v>
+        <v>64</v>
       </c>
       <c r="K35" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>69</v>
+        <v>221</v>
+      </c>
+      <c r="C36" t="s">
+        <v>237</v>
       </c>
       <c r="D36">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="E36">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="G36" t="s">
-        <v>78</v>
+        <v>66</v>
       </c>
       <c r="J36" t="s">
-        <v>16</v>
+        <v>67</v>
       </c>
       <c r="K36" t="s">
-        <v>79</v>
+        <v>65</v>
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>69</v>
+        <v>221</v>
+      </c>
+      <c r="C37" t="s">
+        <v>237</v>
       </c>
       <c r="D37">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E37">
-        <v>2019</v>
+        <v>2021</v>
       </c>
       <c r="G37" t="s">
-        <v>80</v>
+        <v>68</v>
       </c>
       <c r="J37" t="s">
-        <v>77</v>
+        <v>64</v>
       </c>
       <c r="K37" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>152</v>
+        <v>221</v>
+      </c>
+      <c r="C38" t="s">
+        <v>201</v>
+      </c>
+      <c r="D38">
+        <v>5</v>
       </c>
       <c r="E38">
         <v>2021</v>
       </c>
       <c r="G38" t="s">
-        <v>176</v>
-      </c>
-      <c r="H38" t="s">
-        <v>162</v>
+        <v>69</v>
+      </c>
+      <c r="J38" t="s">
+        <v>64</v>
       </c>
       <c r="K38" t="s">
-        <v>170</v>
+        <v>65</v>
       </c>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>152</v>
+        <v>221</v>
+      </c>
+      <c r="C39" t="s">
+        <v>237</v>
+      </c>
+      <c r="D39">
+        <v>6</v>
       </c>
       <c r="E39">
         <v>2021</v>
       </c>
       <c r="G39" t="s">
-        <v>175</v>
-      </c>
-      <c r="H39" t="s">
-        <v>177</v>
+        <v>70</v>
+      </c>
+      <c r="J39" t="s">
+        <v>71</v>
       </c>
       <c r="K39" t="s">
-        <v>170</v>
+        <v>65</v>
       </c>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>152</v>
+        <v>221</v>
+      </c>
+      <c r="C40" t="s">
+        <v>201</v>
+      </c>
+      <c r="D40">
+        <v>7</v>
       </c>
       <c r="E40">
         <v>2020</v>
       </c>
       <c r="G40" t="s">
-        <v>174</v>
-      </c>
-      <c r="H40" t="s">
-        <v>177</v>
+        <v>72</v>
+      </c>
+      <c r="J40" t="s">
+        <v>13</v>
       </c>
       <c r="K40" t="s">
-        <v>185</v>
+        <v>73</v>
       </c>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>152</v>
+        <v>221</v>
+      </c>
+      <c r="C41" t="s">
+        <v>237</v>
+      </c>
+      <c r="D41">
+        <v>8</v>
       </c>
       <c r="E41">
-        <v>2020</v>
+        <v>2019</v>
       </c>
       <c r="G41" t="s">
-        <v>154</v>
-      </c>
-      <c r="H41" t="s">
-        <v>162</v>
+        <v>74</v>
+      </c>
+      <c r="J41" t="s">
+        <v>71</v>
       </c>
       <c r="K41" t="s">
-        <v>168</v>
+        <v>65</v>
       </c>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>152</v>
+        <v>143</v>
+      </c>
+      <c r="C42" t="s">
+        <v>201</v>
       </c>
       <c r="E42">
-        <v>2019</v>
+        <v>2022</v>
       </c>
       <c r="G42" t="s">
-        <v>80</v>
+        <v>220</v>
       </c>
       <c r="H42" t="s">
-        <v>163</v>
+        <v>154</v>
       </c>
       <c r="K42" t="s">
-        <v>169</v>
+        <v>222</v>
       </c>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>152</v>
+        <v>143</v>
+      </c>
+      <c r="C43" t="s">
+        <v>201</v>
       </c>
       <c r="E43">
-        <v>2019</v>
+        <v>2021</v>
       </c>
       <c r="G43" t="s">
-        <v>155</v>
+        <v>167</v>
       </c>
       <c r="H43" t="s">
-        <v>164</v>
+        <v>153</v>
       </c>
       <c r="K43" t="s">
-        <v>170</v>
+        <v>161</v>
       </c>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>152</v>
+        <v>143</v>
+      </c>
+      <c r="C44" t="s">
+        <v>201</v>
       </c>
       <c r="E44">
-        <v>2019</v>
+        <v>2021</v>
       </c>
       <c r="G44" t="s">
-        <v>156</v>
+        <v>166</v>
       </c>
       <c r="H44" t="s">
-        <v>165</v>
+        <v>168</v>
       </c>
       <c r="K44" t="s">
-        <v>153</v>
+        <v>161</v>
       </c>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>152</v>
+        <v>143</v>
+      </c>
+      <c r="C45" t="s">
+        <v>201</v>
       </c>
       <c r="E45">
+        <v>2020</v>
+      </c>
+      <c r="G45" t="s">
+        <v>165</v>
+      </c>
+      <c r="H45" t="s">
+        <v>168</v>
+      </c>
+      <c r="K45" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>143</v>
+      </c>
+      <c r="C46" t="s">
+        <v>201</v>
+      </c>
+      <c r="E46">
+        <v>2020</v>
+      </c>
+      <c r="G46" t="s">
+        <v>145</v>
+      </c>
+      <c r="H46" t="s">
+        <v>153</v>
+      </c>
+      <c r="K46" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>143</v>
+      </c>
+      <c r="C47" t="s">
+        <v>237</v>
+      </c>
+      <c r="E47">
         <v>2019</v>
       </c>
-      <c r="G45" t="s">
-        <v>157</v>
-      </c>
-      <c r="H45" t="s">
-        <v>166</v>
-      </c>
-      <c r="K45" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="46" spans="1:11" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
-        <v>152</v>
-      </c>
-      <c r="E46">
-        <v>2018</v>
-      </c>
-      <c r="G46" t="s">
-        <v>158</v>
-      </c>
-      <c r="H46" t="s">
-        <v>166</v>
-      </c>
-      <c r="K46" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="47" spans="1:11" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
-        <v>152</v>
-      </c>
-      <c r="E47">
-        <v>2018</v>
-      </c>
       <c r="G47" t="s">
-        <v>159</v>
+        <v>74</v>
       </c>
       <c r="H47" t="s">
-        <v>163</v>
+        <v>154</v>
       </c>
       <c r="K47" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="48" spans="1:11" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>152</v>
+        <v>143</v>
+      </c>
+      <c r="C48" t="s">
+        <v>237</v>
       </c>
       <c r="E48">
-        <v>2017</v>
+        <v>2019</v>
       </c>
       <c r="G48" t="s">
-        <v>160</v>
+        <v>146</v>
       </c>
       <c r="H48" t="s">
-        <v>167</v>
+        <v>155</v>
       </c>
       <c r="K48" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="49" spans="1:12" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>152</v>
+        <v>143</v>
+      </c>
+      <c r="C49" t="s">
+        <v>237</v>
       </c>
       <c r="E49">
-        <v>2017</v>
+        <v>2019</v>
       </c>
       <c r="G49" t="s">
-        <v>161</v>
+        <v>147</v>
       </c>
       <c r="H49" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="K49" t="s">
-        <v>172</v>
+        <v>144</v>
       </c>
     </row>
     <row r="50" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>81</v>
-      </c>
-      <c r="D50">
-        <v>1</v>
+        <v>143</v>
+      </c>
+      <c r="C50" t="s">
+        <v>201</v>
       </c>
       <c r="E50">
-        <v>2020</v>
+        <v>2019</v>
       </c>
       <c r="G50" t="s">
-        <v>140</v>
-      </c>
-      <c r="I50" t="s">
-        <v>141</v>
-      </c>
-      <c r="J50" t="s">
-        <v>16</v>
-      </c>
-      <c r="L50" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
+        <v>148</v>
+      </c>
+      <c r="H50" t="s">
+        <v>157</v>
+      </c>
+      <c r="K50" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="51" spans="1:12" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>81</v>
-      </c>
-      <c r="D51">
-        <v>2</v>
+        <v>143</v>
+      </c>
+      <c r="C51" t="s">
+        <v>201</v>
       </c>
       <c r="E51">
         <v>2018</v>
       </c>
       <c r="G51" t="s">
-        <v>13</v>
-      </c>
-      <c r="I51" t="s">
-        <v>15</v>
-      </c>
-      <c r="J51" t="s">
-        <v>16</v>
-      </c>
-      <c r="L51" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
+        <v>149</v>
+      </c>
+      <c r="H51" t="s">
+        <v>157</v>
+      </c>
+      <c r="K51" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="52" spans="1:12" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>81</v>
-      </c>
-      <c r="D52">
-        <v>3</v>
+        <v>143</v>
+      </c>
+      <c r="C52" t="s">
+        <v>237</v>
       </c>
       <c r="E52">
         <v>2018</v>
       </c>
       <c r="G52" t="s">
-        <v>84</v>
+        <v>150</v>
       </c>
       <c r="H52" t="s">
-        <v>85</v>
-      </c>
-      <c r="I52" t="s">
-        <v>15</v>
-      </c>
-      <c r="J52" t="s">
-        <v>16</v>
-      </c>
-      <c r="L52" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
+        <v>154</v>
+      </c>
+      <c r="K52" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="53" spans="1:12" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>81</v>
-      </c>
-      <c r="D53">
-        <v>4</v>
+        <v>143</v>
+      </c>
+      <c r="C53" t="s">
+        <v>237</v>
       </c>
       <c r="E53">
         <v>2017</v>
       </c>
       <c r="G53" t="s">
-        <v>87</v>
-      </c>
-      <c r="I53" t="s">
-        <v>88</v>
-      </c>
-      <c r="J53" t="s">
-        <v>25</v>
-      </c>
-      <c r="L53" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
+        <v>151</v>
+      </c>
+      <c r="H53" t="s">
+        <v>158</v>
+      </c>
+      <c r="K53" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="54" spans="1:12" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>81</v>
-      </c>
-      <c r="D54">
-        <v>5</v>
+        <v>143</v>
+      </c>
+      <c r="C54" t="s">
+        <v>237</v>
       </c>
       <c r="E54">
         <v>2017</v>
       </c>
       <c r="G54" t="s">
-        <v>90</v>
-      </c>
-      <c r="I54" t="s">
-        <v>91</v>
-      </c>
-      <c r="J54" t="s">
-        <v>25</v>
-      </c>
-      <c r="L54" t="s">
-        <v>92</v>
+        <v>152</v>
+      </c>
+      <c r="H54" t="s">
+        <v>153</v>
+      </c>
+      <c r="K54" t="s">
+        <v>163</v>
       </c>
     </row>
     <row r="55" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>93</v>
+        <v>228</v>
+      </c>
+      <c r="C55" t="s">
+        <v>237</v>
+      </c>
+      <c r="D55">
+        <v>1</v>
       </c>
       <c r="E55">
-        <v>2021</v>
+        <v>2020</v>
       </c>
       <c r="G55" t="s">
-        <v>100</v>
+        <v>132</v>
       </c>
       <c r="I55" t="s">
-        <v>94</v>
-      </c>
-      <c r="K55" t="s">
-        <v>104</v>
+        <v>133</v>
+      </c>
+      <c r="J55" t="s">
+        <v>13</v>
       </c>
       <c r="L55" t="s">
-        <v>96</v>
+        <v>75</v>
       </c>
     </row>
     <row r="56" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>93</v>
+        <v>228</v>
+      </c>
+      <c r="C56" t="s">
+        <v>237</v>
+      </c>
+      <c r="D56">
+        <v>2</v>
       </c>
       <c r="E56">
-        <v>2021</v>
+        <v>2018</v>
       </c>
       <c r="G56" t="s">
-        <v>97</v>
+        <v>10</v>
       </c>
       <c r="I56" t="s">
-        <v>94</v>
-      </c>
-      <c r="K56" t="s">
-        <v>98</v>
+        <v>12</v>
+      </c>
+      <c r="J56" t="s">
+        <v>13</v>
       </c>
       <c r="L56" t="s">
-        <v>99</v>
+        <v>76</v>
       </c>
     </row>
     <row r="57" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>93</v>
+        <v>228</v>
+      </c>
+      <c r="C57" t="s">
+        <v>237</v>
+      </c>
+      <c r="D57">
+        <v>3</v>
       </c>
       <c r="E57">
-        <v>2021</v>
+        <v>2018</v>
       </c>
       <c r="G57" t="s">
-        <v>101</v>
+        <v>77</v>
+      </c>
+      <c r="H57" t="s">
+        <v>78</v>
       </c>
       <c r="I57" t="s">
-        <v>94</v>
-      </c>
-      <c r="K57" t="s">
-        <v>95</v>
+        <v>12</v>
+      </c>
+      <c r="J57" t="s">
+        <v>13</v>
       </c>
       <c r="L57" t="s">
-        <v>96</v>
+        <v>79</v>
       </c>
     </row>
     <row r="58" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>93</v>
+        <v>228</v>
+      </c>
+      <c r="C58" t="s">
+        <v>237</v>
+      </c>
+      <c r="D58">
+        <v>4</v>
       </c>
       <c r="E58">
-        <v>2019</v>
+        <v>2017</v>
       </c>
       <c r="G58" t="s">
-        <v>31</v>
+        <v>80</v>
       </c>
       <c r="I58" t="s">
-        <v>94</v>
-      </c>
-      <c r="K58" t="s">
-        <v>103</v>
+        <v>81</v>
+      </c>
+      <c r="J58" t="s">
+        <v>21</v>
       </c>
       <c r="L58" t="s">
-        <v>102</v>
+        <v>82</v>
       </c>
     </row>
     <row r="59" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>105</v>
+        <v>228</v>
+      </c>
+      <c r="C59" t="s">
+        <v>237</v>
+      </c>
+      <c r="D59">
+        <v>5</v>
       </c>
       <c r="E59">
-        <v>2021</v>
+        <v>2017</v>
       </c>
       <c r="G59" t="s">
-        <v>110</v>
+        <v>83</v>
       </c>
       <c r="I59" t="s">
-        <v>94</v>
-      </c>
-      <c r="K59" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
+        <v>84</v>
+      </c>
+      <c r="J59" t="s">
+        <v>21</v>
+      </c>
+      <c r="L59" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="60" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>105</v>
+        <v>86</v>
+      </c>
+      <c r="C60" t="s">
+        <v>201</v>
       </c>
       <c r="E60">
-        <v>2019</v>
+        <v>2022</v>
       </c>
       <c r="G60" t="s">
-        <v>31</v>
-      </c>
-      <c r="H60" t="s">
-        <v>107</v>
+        <v>223</v>
       </c>
       <c r="I60" t="s">
-        <v>32</v>
+        <v>224</v>
       </c>
       <c r="J60" t="s">
-        <v>25</v>
+        <v>225</v>
+      </c>
+      <c r="K60" t="s">
+        <v>226</v>
+      </c>
+      <c r="L60" s="1" t="s">
+        <v>227</v>
       </c>
     </row>
     <row r="61" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>105</v>
+        <v>86</v>
+      </c>
+      <c r="C61" t="s">
+        <v>201</v>
       </c>
       <c r="E61">
-        <v>2019</v>
+        <v>2021</v>
       </c>
       <c r="G61" t="s">
-        <v>111</v>
-      </c>
-      <c r="H61" t="s">
-        <v>112</v>
+        <v>93</v>
       </c>
       <c r="I61" t="s">
-        <v>182</v>
-      </c>
-      <c r="J61" t="s">
-        <v>70</v>
+        <v>87</v>
+      </c>
+      <c r="K61" t="s">
+        <v>97</v>
+      </c>
+      <c r="L61" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="62" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>105</v>
+        <v>86</v>
+      </c>
+      <c r="C62" t="s">
+        <v>201</v>
       </c>
       <c r="E62">
-        <v>2018</v>
+        <v>2021</v>
       </c>
       <c r="G62" t="s">
-        <v>183</v>
-      </c>
-      <c r="H62" t="s">
-        <v>106</v>
+        <v>90</v>
       </c>
       <c r="I62" t="s">
-        <v>138</v>
-      </c>
-      <c r="J62" t="s">
-        <v>16</v>
+        <v>87</v>
+      </c>
+      <c r="K62" t="s">
+        <v>91</v>
+      </c>
+      <c r="L62" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="63" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>105</v>
+        <v>86</v>
+      </c>
+      <c r="C63" t="s">
+        <v>201</v>
       </c>
       <c r="E63">
-        <v>2018</v>
+        <v>2021</v>
       </c>
       <c r="G63" t="s">
-        <v>111</v>
-      </c>
-      <c r="H63" t="s">
-        <v>112</v>
+        <v>94</v>
       </c>
       <c r="I63" t="s">
-        <v>184</v>
-      </c>
-      <c r="J63" t="s">
-        <v>113</v>
+        <v>87</v>
+      </c>
+      <c r="K63" t="s">
+        <v>88</v>
+      </c>
+      <c r="L63" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="64" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>105</v>
+        <v>86</v>
+      </c>
+      <c r="C64" t="s">
+        <v>201</v>
       </c>
       <c r="E64">
-        <v>2018</v>
+        <v>2019</v>
       </c>
       <c r="G64" t="s">
-        <v>110</v>
-      </c>
-      <c r="H64" t="s">
-        <v>106</v>
+        <v>27</v>
       </c>
       <c r="I64" t="s">
-        <v>108</v>
-      </c>
-      <c r="J64" t="s">
-        <v>109</v>
+        <v>87</v>
+      </c>
+      <c r="K64" t="s">
+        <v>96</v>
+      </c>
+      <c r="L64" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="65" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>114</v>
-      </c>
-      <c r="E65" t="s">
-        <v>12</v>
+        <v>98</v>
+      </c>
+      <c r="C65" t="s">
+        <v>201</v>
+      </c>
+      <c r="E65">
+        <v>2022</v>
       </c>
       <c r="G65" t="s">
-        <v>117</v>
+        <v>229</v>
+      </c>
+      <c r="H65" t="s">
+        <v>99</v>
+      </c>
+      <c r="I65" t="s">
+        <v>130</v>
+      </c>
+      <c r="J65" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="66" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>114</v>
+        <v>98</v>
+      </c>
+      <c r="C66" t="s">
+        <v>201</v>
       </c>
       <c r="E66">
-        <v>2020</v>
-      </c>
-      <c r="F66">
         <v>2021</v>
       </c>
       <c r="G66" t="s">
-        <v>115</v>
+        <v>103</v>
+      </c>
+      <c r="H66" t="s">
+        <v>99</v>
+      </c>
+      <c r="I66" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="67" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>114</v>
+        <v>98</v>
+      </c>
+      <c r="C67" t="s">
+        <v>201</v>
       </c>
       <c r="E67">
         <v>2019</v>
       </c>
       <c r="G67" t="s">
-        <v>116</v>
+        <v>27</v>
+      </c>
+      <c r="H67" t="s">
+        <v>100</v>
+      </c>
+      <c r="I67" t="s">
+        <v>28</v>
+      </c>
+      <c r="J67" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="68" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>114</v>
+        <v>98</v>
+      </c>
+      <c r="C68" t="s">
+        <v>201</v>
       </c>
       <c r="E68">
         <v>2019</v>
       </c>
       <c r="G68" t="s">
-        <v>137</v>
+        <v>104</v>
+      </c>
+      <c r="H68" t="s">
+        <v>105</v>
       </c>
       <c r="I68" t="s">
-        <v>138</v>
+        <v>173</v>
       </c>
       <c r="J68" t="s">
-        <v>16</v>
+        <v>64</v>
       </c>
     </row>
     <row r="69" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>114</v>
+        <v>98</v>
+      </c>
+      <c r="C69" t="s">
+        <v>237</v>
       </c>
       <c r="E69">
-        <v>2019</v>
+        <v>2018</v>
       </c>
       <c r="G69" t="s">
-        <v>135</v>
+        <v>174</v>
+      </c>
+      <c r="H69" t="s">
+        <v>99</v>
       </c>
       <c r="I69" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="J69" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
     <row r="70" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>114</v>
+        <v>98</v>
+      </c>
+      <c r="C70" t="s">
+        <v>237</v>
       </c>
       <c r="E70">
         <v>2018</v>
       </c>
-      <c r="F70">
-        <v>2019</v>
-      </c>
       <c r="G70" t="s">
-        <v>134</v>
+        <v>104</v>
+      </c>
+      <c r="H70" t="s">
+        <v>105</v>
+      </c>
+      <c r="I70" t="s">
+        <v>175</v>
+      </c>
+      <c r="J70" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="71" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>114</v>
+        <v>98</v>
+      </c>
+      <c r="C71" t="s">
+        <v>237</v>
       </c>
       <c r="E71">
         <v>2018</v>
       </c>
       <c r="G71" t="s">
-        <v>118</v>
+        <v>103</v>
+      </c>
+      <c r="H71" t="s">
+        <v>99</v>
+      </c>
+      <c r="I71" t="s">
+        <v>101</v>
+      </c>
+      <c r="J71" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="72" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>119</v>
-      </c>
-      <c r="E72">
-        <v>2019</v>
+        <v>107</v>
+      </c>
+      <c r="C72" t="s">
+        <v>201</v>
+      </c>
+      <c r="E72" t="s">
+        <v>230</v>
+      </c>
+      <c r="F72" t="s">
+        <v>231</v>
       </c>
       <c r="G72" t="s">
-        <v>120</v>
-      </c>
-      <c r="H72" t="s">
-        <v>121</v>
-      </c>
-      <c r="I72" t="s">
-        <v>122</v>
-      </c>
-      <c r="J72" t="s">
-        <v>16</v>
+        <v>110</v>
       </c>
     </row>
     <row r="73" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>119</v>
+        <v>107</v>
+      </c>
+      <c r="C73" t="s">
+        <v>201</v>
       </c>
       <c r="E73">
-        <v>2018</v>
+        <v>2020</v>
+      </c>
+      <c r="F73">
+        <v>2021</v>
       </c>
       <c r="G73" t="s">
-        <v>123</v>
-      </c>
-      <c r="I73" t="s">
-        <v>124</v>
-      </c>
-      <c r="J73" t="s">
-        <v>16</v>
+        <v>108</v>
       </c>
     </row>
     <row r="74" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>178</v>
+        <v>107</v>
+      </c>
+      <c r="C74" t="s">
+        <v>201</v>
       </c>
       <c r="E74">
         <v>2019</v>
       </c>
       <c r="G74" t="s">
-        <v>179</v>
+        <v>109</v>
       </c>
     </row>
     <row r="75" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>178</v>
+        <v>107</v>
+      </c>
+      <c r="C75" t="s">
+        <v>201</v>
       </c>
       <c r="E75">
         <v>2019</v>
       </c>
       <c r="G75" t="s">
-        <v>180</v>
-      </c>
-      <c r="H75" t="s">
-        <v>181</v>
+        <v>129</v>
+      </c>
+      <c r="I75" t="s">
+        <v>130</v>
+      </c>
+      <c r="J75" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="76" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>125</v>
-      </c>
-      <c r="E76" t="s">
+        <v>107</v>
+      </c>
+      <c r="C76" t="s">
+        <v>237</v>
+      </c>
+      <c r="E76">
+        <v>2019</v>
+      </c>
+      <c r="G76" t="s">
         <v>127</v>
       </c>
-      <c r="G76" t="s">
-        <v>126</v>
+      <c r="I76" t="s">
+        <v>128</v>
+      </c>
+      <c r="J76" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="77" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>125</v>
-      </c>
-      <c r="E77" t="s">
-        <v>129</v>
+        <v>107</v>
+      </c>
+      <c r="C77" t="s">
+        <v>237</v>
+      </c>
+      <c r="E77">
+        <v>2018</v>
+      </c>
+      <c r="F77">
+        <v>2019</v>
       </c>
       <c r="G77" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
     <row r="78" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>125</v>
-      </c>
-      <c r="E78" t="s">
-        <v>130</v>
+        <v>107</v>
+      </c>
+      <c r="C78" t="s">
+        <v>201</v>
+      </c>
+      <c r="E78">
+        <v>2018</v>
       </c>
       <c r="G78" t="s">
-        <v>131</v>
+        <v>111</v>
       </c>
     </row>
     <row r="79" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
+        <v>112</v>
+      </c>
+      <c r="C79" t="s">
+        <v>201</v>
+      </c>
+      <c r="E79">
+        <v>2019</v>
+      </c>
+      <c r="G79" t="s">
+        <v>113</v>
+      </c>
+      <c r="H79" t="s">
+        <v>114</v>
+      </c>
+      <c r="I79" t="s">
+        <v>115</v>
+      </c>
+      <c r="J79" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>112</v>
+      </c>
+      <c r="C80" t="s">
+        <v>201</v>
+      </c>
+      <c r="E80">
+        <v>2018</v>
+      </c>
+      <c r="G80" t="s">
+        <v>116</v>
+      </c>
+      <c r="I80" t="s">
+        <v>117</v>
+      </c>
+      <c r="J80" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>169</v>
+      </c>
+      <c r="C81" t="s">
+        <v>201</v>
+      </c>
+      <c r="E81">
+        <v>2019</v>
+      </c>
+      <c r="G81" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>169</v>
+      </c>
+      <c r="C82" t="s">
+        <v>201</v>
+      </c>
+      <c r="E82">
+        <v>2019</v>
+      </c>
+      <c r="G82" t="s">
+        <v>171</v>
+      </c>
+      <c r="H82" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>118</v>
+      </c>
+      <c r="C83" t="s">
+        <v>201</v>
+      </c>
+      <c r="E83" t="s">
+        <v>120</v>
+      </c>
+      <c r="G83" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>118</v>
+      </c>
+      <c r="C84" t="s">
+        <v>201</v>
+      </c>
+      <c r="E84" t="s">
+        <v>122</v>
+      </c>
+      <c r="G84" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>118</v>
+      </c>
+      <c r="C85" t="s">
+        <v>201</v>
+      </c>
+      <c r="E85" t="s">
+        <v>123</v>
+      </c>
+      <c r="G85" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>118</v>
+      </c>
+      <c r="C86" t="s">
+        <v>201</v>
+      </c>
+      <c r="E86" t="s">
+        <v>236</v>
+      </c>
+      <c r="G86" t="s">
         <v>125</v>
-      </c>
-      <c r="E79" t="s">
-        <v>132</v>
-      </c>
-      <c r="G79" t="s">
-        <v>133</v>
       </c>
     </row>
   </sheetData>

</xml_diff>